<commit_message>
add m2019 5 - excel, chmury soultion
</commit_message>
<xml_diff>
--- a/2019 [teoria, praktyka - ponownie]/5 - excel, chmury - old/5.xlsx
+++ b/2019 [teoria, praktyka - ponownie]/5 - excel, chmury - old/5.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20370"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F70A4D-0551-4E06-9E89-681B25770E5D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22DD9CA4-A803-4EC9-A2E6-2AA8467205E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5.1 i 5.2" sheetId="2" r:id="rId1"/>
@@ -354,7 +354,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[m2019-5.xlsx]5.3!Tabela przestawna2</c:name>
+    <c:name>[5.xlsx]5.3!Tabela przestawna2</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -414,7 +414,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="pl-PL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -477,7 +477,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES"/>
+              <a:endParaRPr lang="pl-PL"/>
             </a:p>
           </c:txPr>
           <c:dLblPos val="outEnd"/>
@@ -534,7 +534,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES"/>
+              <a:endParaRPr lang="pl-PL"/>
             </a:p>
           </c:txPr>
           <c:dLblPos val="outEnd"/>
@@ -607,7 +607,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-ES"/>
+                <a:endParaRPr lang="pl-PL"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -742,7 +742,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-ES"/>
+                <a:endParaRPr lang="pl-PL"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -899,7 +899,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES"/>
+              <a:endParaRPr lang="pl-PL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -937,7 +937,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="763019519"/>
@@ -1024,7 +1024,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES"/>
+              <a:endParaRPr lang="pl-PL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1056,7 +1056,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="762603039"/>
@@ -1098,7 +1098,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="pl-PL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1135,7 +1135,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="pl-PL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -29421,7 +29421,7 @@
   <dimension ref="A1:R501"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A281" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I295" sqref="I295"/>
+      <selection activeCell="J302" sqref="J302"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>